<commit_message>
final version (stft part leads to mis classification)
</commit_message>
<xml_diff>
--- a/TSD_C/TSD_PY/sw/applications/transformer_C_approx/docs/transformer_notes.xlsx
+++ b/TSD_C/TSD_PY/sw/applications/transformer_C_approx/docs/transformer_notes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
   <si>
     <t>note in int16_t</t>
   </si>
@@ -303,6 +303,18 @@
   </si>
   <si>
     <t>comp_amp variations (w/o FPU)</t>
+  </si>
+  <si>
+    <t>LOG_AMP_FXP_LUT</t>
+  </si>
+  <si>
+    <t>LOG_AMP_FXP_APPROX</t>
+  </si>
+  <si>
+    <t>all fixed (although log_amp is faulty)</t>
+  </si>
+  <si>
+    <t>logamp_approx_sm_fixed_gelu_pwl</t>
   </si>
 </sst>
 </file>
@@ -1329,12 +1341,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="37"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
+      <c r="B18" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="26">
+        <v>767747770</v>
+      </c>
       <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
+      <c r="F18" s="26">
+        <v>92257</v>
+      </c>
+      <c r="G18" s="26">
+        <v>2229</v>
+      </c>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
       <c r="J18" s="26"/>
@@ -1345,11 +1367,19 @@
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="37"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="C19" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="26">
+        <v>728430738</v>
+      </c>
       <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="26">
+        <v>215213</v>
+      </c>
+      <c r="G19" s="26">
+        <v>24505</v>
+      </c>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
       <c r="J19" s="26"/>
@@ -1359,8 +1389,12 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="37"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>81</v>
+      </c>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
@@ -1375,11 +1409,19 @@
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="37"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="C21" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="26">
+        <v>294178509</v>
+      </c>
       <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
+      <c r="F21" s="26">
+        <v>208442</v>
+      </c>
+      <c r="G21" s="26">
+        <v>19958</v>
+      </c>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
       <c r="J21" s="26"/>

</xml_diff>